<commit_message>
Adding test case 633. Update members with invalid relation value and fixing member relations in Excels
</commit_message>
<xml_diff>
--- a/test_files/Code_list_calc_hier_members.xlsx
+++ b/test_files/Code_list_calc_hier_members.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21723"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E074C738-F565-483A-8051-D86745217307}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC56E2BD-9044-4250-96E3-6BC595B27CFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="4" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="156">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -410,6 +410,9 @@
     <t>Member2</t>
   </si>
   <si>
+    <t>code:testcode01</t>
+  </si>
+  <si>
     <t>Jäsen3</t>
   </si>
   <si>
@@ -428,12 +431,18 @@
     <t>Member5</t>
   </si>
   <si>
+    <t>code:testcode04</t>
+  </si>
+  <si>
     <t>Jäsen6</t>
   </si>
   <si>
     <t>Member6</t>
   </si>
   <si>
+    <t>code:testcode05</t>
+  </si>
+  <si>
     <t>Jäsen7</t>
   </si>
   <si>
@@ -468,6 +477,18 @@
   </si>
   <si>
     <t>&lt;=</t>
+  </si>
+  <si>
+    <t>code:testcode08</t>
+  </si>
+  <si>
+    <t>code:testcode09</t>
+  </si>
+  <si>
+    <t>code:testcode12</t>
+  </si>
+  <si>
+    <t>code:testcode13</t>
   </si>
   <si>
     <t>Jäsen8</t>
@@ -4821,7 +4842,9 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -4884,7 +4907,7 @@
         <v>126</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="3">
@@ -4899,13 +4922,13 @@
         <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="3">
@@ -4920,10 +4943,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="5"/>
@@ -4939,13 +4962,13 @@
         <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>43</v>
+        <v>134</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="3">
@@ -4960,13 +4983,13 @@
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>137</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="3">
@@ -4981,10 +5004,10 @@
         <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="5"/>
@@ -4997,13 +5020,13 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="5"/>
@@ -5016,13 +5039,13 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="5"/>
@@ -6039,8 +6062,8 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6050,10 +6073,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>121</v>
@@ -6079,10 +6102,10 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>54</v>
@@ -6106,10 +6129,10 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>57</v>
@@ -6121,7 +6144,7 @@
         <v>126</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="3">
@@ -6133,22 +6156,22 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="3">
@@ -6160,19 +6183,19 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="5"/>
@@ -6185,19 +6208,19 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="5"/>
@@ -6210,22 +6233,22 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>152</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="3">
@@ -6237,22 +6260,22 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="3">
@@ -6264,22 +6287,22 @@
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="3">
@@ -6291,19 +6314,19 @@
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="5"/>

</xml_diff>